<commit_message>
Finish Market Random Call
</commit_message>
<xml_diff>
--- a/excels/market.xlsx
+++ b/excels/market.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="market_item" sheetId="1" r:id="rId1"/>
     <sheet name="market_level_resource" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,11 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>序号</t>
   </si>
   <si>
+    <t>market 物品商店 ability 技能商店</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -52,6 +54,9 @@
     <t>weight</t>
   </si>
   <si>
+    <t>tag</t>
+  </si>
+  <si>
     <t>normalAttack</t>
   </si>
   <si>
@@ -61,28 +66,52 @@
     <t>test_gloves.png</t>
   </si>
   <si>
+    <t>market</t>
+  </si>
+  <si>
     <t>normalAttack2</t>
   </si>
   <si>
     <t>market_item_CN_normalAttack2</t>
   </si>
   <si>
-    <t>market 物品商店 ability 技能商店</t>
+    <t>normalAttack3</t>
+  </si>
+  <si>
+    <t>market_item_CN_normalAttack3</t>
+  </si>
+  <si>
+    <t>normalAttack4</t>
+  </si>
+  <si>
+    <t>market_item_CN_normalAttack4</t>
+  </si>
+  <si>
+    <t>normalAttack5</t>
+  </si>
+  <si>
+    <t>market_item_CN_normalAttack5</t>
+  </si>
+  <si>
+    <t>normalAttack6</t>
+  </si>
+  <si>
+    <t>market_item_CN_normalAttack6</t>
+  </si>
+  <si>
+    <t>normalAttack7</t>
+  </si>
+  <si>
+    <t>market_item_CN_normalAttack7</t>
   </si>
   <si>
     <t>gold 金币 | lumber 木材</t>
   </si>
   <si>
-    <t>tag</t>
-  </si>
-  <si>
     <t>val</t>
   </si>
   <si>
     <t>resource</t>
-  </si>
-  <si>
-    <t>market</t>
   </si>
   <si>
     <t>gold</t>
@@ -1016,13 +1045,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="15.2727272727273" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -1030,46 +1059,52 @@
     <col min="4" max="4" width="18.5454545454545" customWidth="1"/>
     <col min="5" max="5" width="22.5454545454545" customWidth="1"/>
     <col min="6" max="6" width="20.5454545454545" customWidth="1"/>
-    <col min="7" max="7" width="14.9090909090909" customWidth="1"/>
+    <col min="7" max="7" width="54.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1077,25 +1112,146 @@
       <c r="F3">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
         <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1267,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1125,30 +1281,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1159,13 +1315,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1173,21 +1329,4 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>